<commit_message>
update productlist anda productdetail
</commit_message>
<xml_diff>
--- a/app/public/json/prodata.xlsx
+++ b/app/public/json/prodata.xlsx
@@ -8,19 +8,21 @@
   </bookViews>
   <sheets>
     <sheet name="男性健康滋补" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="女性健康面容" sheetId="2" r:id="rId2"/>
+    <sheet name="综合健康护理" sheetId="3" r:id="rId3"/>
+    <sheet name="舒缓调理" sheetId="4" r:id="rId4"/>
+    <sheet name="提升免疫力" sheetId="5" r:id="rId5"/>
+    <sheet name="美容养颜" sheetId="6" r:id="rId6"/>
+    <sheet name="内脏保健" sheetId="7" r:id="rId7"/>
+    <sheet name="骨骼健康" sheetId="8" r:id="rId8"/>
+    <sheet name="明目健脑" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
-  <si>
-    <t>manyuemei.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,15 +68,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>男性健康滋补</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>女性美容</t>
+    <t>manyuemei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>img_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pro_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>袋鼠精</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>daishujing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kangaroo Essence袋鼠精</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>90粒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每一粒含6000mg袋鼠肉提取精华，功效更强！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>袋鼠粉（600mg/粒）、角豆荚、维生素C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男性肾虚腰酸，性功能减退，病后体虚，精力不济，生活不规律</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保肝宁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baoganning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60粒/180粒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姜黄，葛根</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经常饮酒、吸烟、肝火旺盛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>适合有肝脏问题困扰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Health Complex保肝宁</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -82,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +165,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,11 +197,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -428,129 +501,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="14.375" customWidth="1"/>
-    <col min="2" max="2" width="29.625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="21.75" customWidth="1"/>
-    <col min="5" max="5" width="22.375" customWidth="1"/>
-    <col min="6" max="6" width="27.375" customWidth="1"/>
+    <col min="2" max="2" width="44.375" customWidth="1"/>
+    <col min="3" max="3" width="29.625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="21.75" customWidth="1"/>
+    <col min="6" max="6" width="22.375" customWidth="1"/>
+    <col min="7" max="7" width="27.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="14.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="24.75" customHeight="1">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25">
       <c r="A11" s="1"/>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
+      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -560,6 +608,196 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="16.25" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="14.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G42" sqref="G42:H42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
@@ -572,11 +810,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>

</xml_diff>